<commit_message>
Updated reports and Week 12.docx
Added some format for reports (Exception and detail report)
Week 12.docx completed
</commit_message>
<xml_diff>
--- a/Week 12/Reports.xlsx
+++ b/Week 12/Reports.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22010"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B101A6-4028-4BD3-81E5-731B4CEF742F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA2A3293-1E28-4F00-91C6-90B9F2FC1F3C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="1185" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reservation Report" sheetId="1" r:id="rId1"/>
     <sheet name="Long-time Unpaid Report" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
   <si>
     <t>              Perpustakaan Negara Malaysia</t>
   </si>
@@ -36,6 +32,12 @@
     <t>Reservation Report on May 2019</t>
   </si>
   <si>
+    <t>Generated on 14/8/2019</t>
+  </si>
+  <si>
+    <t>Page 1 of 2</t>
+  </si>
+  <si>
     <t>Reserve Date</t>
   </si>
   <si>
@@ -216,6 +218,9 @@
     <t>000014</t>
   </si>
   <si>
+    <t>Page 2 of 2</t>
+  </si>
+  <si>
     <t>R0202</t>
   </si>
   <si>
@@ -246,9 +251,27 @@
     <t>MSNF91384</t>
   </si>
   <si>
+    <t>Number of Reservation on May:</t>
+  </si>
+  <si>
+    <t>22 Books</t>
+  </si>
+  <si>
     <t>#000001</t>
   </si>
   <si>
+    <t xml:space="preserve">              Perpustakaan Negara Malaysia</t>
+  </si>
+  <si>
+    <t>Report of Late Unpaid Fines over 7 Days for</t>
+  </si>
+  <si>
+    <t>the Month Ended March, April and May 2019</t>
+  </si>
+  <si>
+    <t>Page 1 of 1</t>
+  </si>
+  <si>
     <t>Month</t>
   </si>
   <si>
@@ -301,15 +324,6 @@
   </si>
   <si>
     <t>Grand total</t>
-  </si>
-  <si>
-    <t>Late Unpaid Fines Over 7 days</t>
-  </si>
-  <si>
-    <t>the Month Ended March, April and May 2019</t>
-  </si>
-  <si>
-    <t>Report of Late Unpaid Fines over 7 Days for</t>
   </si>
 </sst>
 </file>
@@ -320,7 +334,7 @@
     <numFmt numFmtId="164" formatCode="[$-809]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +347,18 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -342,7 +368,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -359,35 +385,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -398,46 +395,46 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -467,14 +464,14 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="2" name="">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB739BE-B30F-4C90-A51F-46627AE389EA}"/>
@@ -523,7 +520,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="3" name="">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D2976C0-33CC-445C-95F7-15EC573D4BAA}"/>
@@ -857,20 +854,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="21.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="7" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" customWidth="1"/>
     <col min="11" max="12" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21.75" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -882,7 +881,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21.75" customHeight="1">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -892,7 +891,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="21.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
@@ -904,478 +903,531 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:8" ht="21.75" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="10"/>
+      <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B6" s="2">
         <v>43586</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4">
+      <c r="D6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
         <v>43589</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G6" s="3">
         <v>43620</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+    <row r="7" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B7" s="2">
         <v>43587</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4">
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="3">
         <v>43591</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G7" s="3">
         <v>43622</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+    <row r="8" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B8" s="2">
         <v>43588</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="4">
+      <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3">
         <v>43594</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G8" s="3">
         <v>43625</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+    <row r="9" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B9" s="2">
         <v>43589</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4">
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3">
         <v>43592</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G9" s="3">
         <v>43623</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+    <row r="10" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B10" s="2">
         <v>43591</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="4">
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3">
         <v>43593</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G10" s="3">
         <v>43624</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>43594</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="4">
-        <v>43597</v>
-      </c>
-      <c r="G10" s="4">
-        <v>43628</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="21.75" customHeight="1">
       <c r="B11" s="2">
         <v>43594</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="4">
-        <v>43595</v>
-      </c>
-      <c r="G11" s="4">
-        <v>43626</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="3">
+        <v>43597</v>
+      </c>
+      <c r="G11" s="3">
+        <v>43628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21.75" customHeight="1">
       <c r="B12" s="2">
         <v>43594</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="3">
+        <v>43595</v>
+      </c>
+      <c r="G12" s="3">
+        <v>43626</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B13" s="2">
+        <v>43594</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="4">
+      <c r="D13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="3">
         <v>43602</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G13" s="3">
         <v>43633</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+    <row r="14" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B14" s="2">
         <v>43596</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="4">
+      <c r="D14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="3">
         <v>43598</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G14" s="3">
         <v>43629</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+    <row r="15" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B15" s="2">
         <v>43597</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="C15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="4">
+      <c r="D15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="3">
         <v>43603</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G15" s="3">
         <v>43634</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+    <row r="16" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B16" s="2">
         <v>43599</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="4">
+      <c r="D16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="3">
         <v>43604</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="3">
         <v>43635</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>43600</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="4">
-        <v>43605</v>
-      </c>
-      <c r="G16" s="4">
-        <v>43636</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="21.75" customHeight="1">
       <c r="B17" s="2">
         <v>43600</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="3">
+        <v>43605</v>
+      </c>
+      <c r="G17" s="3">
+        <v>43636</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B18" s="2">
+        <v>43600</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="4">
+      <c r="D18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3">
         <v>43607</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G18" s="3">
         <v>43638</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+    <row r="19" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B19" s="2">
         <v>43604</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="C19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="4">
+      <c r="D19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="3">
         <v>43608</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G19" s="3">
         <v>43639</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+    <row r="20" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B20" s="2">
         <v>43605</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="4">
+      <c r="D20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3">
         <v>43609</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G20" s="3">
         <v>43640</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+    <row r="21" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B21" s="2">
         <v>43606</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="C21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="4">
+      <c r="D21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="3">
         <v>43612</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G21" s="3">
         <v>43643</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+    <row r="22" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B22" s="2">
         <v>43607</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="C22" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="4">
+      <c r="D22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="3">
         <v>43612</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G22" s="3">
         <v>43643</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+    <row r="23" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B23" s="2">
         <v>43612</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="C23" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="4">
+      <c r="D23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="3">
         <v>43613</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G23" s="3">
         <v>43644</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+    <row r="24" spans="1:8" ht="21.75" customHeight="1">
+      <c r="A24" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="G24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B26" s="2">
         <v>43613</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="4">
+      <c r="C26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="3">
         <v>43615</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G26" s="3">
         <v>43646</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
+    <row r="27" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B27" s="2">
         <v>43614</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="4">
+      <c r="C27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="3">
         <v>43616</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G27" s="3">
         <v>43647</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
+    <row r="28" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B28" s="2">
         <v>43614</v>
       </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="4">
+      <c r="C28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="3">
         <v>43648</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
+    <row r="29" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B29" s="2">
         <v>43614</v>
       </c>
-      <c r="C26" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="4">
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="3">
         <v>43648</v>
       </c>
     </row>
-    <row r="1048576" spans="5:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B31" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1048576" spans="5:5" ht="21.75" customHeight="1">
       <c r="E1048576" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F5:G14">
-    <sortCondition ref="F5:F14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F6:G15">
+    <sortCondition ref="F6:F15"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1387,10 +1439,10 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
@@ -1398,9 +1450,9 @@
     <col min="5" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21.75" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1410,7 +1462,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21.75" customHeight="1">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1420,213 +1472,234 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="1:8" ht="21.75" customHeight="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" ht="21.75" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" ht="21.75" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="G5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="15">
+        <v>8</v>
+      </c>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" ht="21.75" customHeight="1">
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="15">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" ht="21.75" customHeight="1">
+      <c r="C9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="14">
+        <v>9</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="21.75" customHeight="1">
+      <c r="C10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="8">
+        <v>3</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" ht="21.75" customHeight="1">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" ht="21.75" customHeight="1">
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="15">
+        <v>7</v>
+      </c>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" ht="21.75" customHeight="1">
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="15">
+        <v>7</v>
+      </c>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" ht="21.75" customHeight="1">
+      <c r="C14" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="F14" s="15">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" ht="21.75" customHeight="1">
+      <c r="C15" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="14">
+        <v>4</v>
+      </c>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" ht="21.75" customHeight="1">
+      <c r="C16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="8">
+        <v>4</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="2:7" ht="21.75" customHeight="1">
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="2:7" ht="21.75" customHeight="1">
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="15">
         <v>8</v>
       </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="2:7" ht="21.75" customHeight="1">
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="15">
+        <v>9</v>
+      </c>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="2:7" ht="21.75" customHeight="1">
+      <c r="C20" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="14">
+        <v>15</v>
+      </c>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="2:7" ht="21.75" customHeight="1">
+      <c r="C21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="21.75" customHeight="1"/>
+    <row r="23" spans="2:7" ht="21.75" customHeight="1">
+      <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="8">
         <v>10</v>
       </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="11">
-        <v>9</v>
-      </c>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="6">
-        <v>7</v>
-      </c>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="6">
-        <v>7</v>
-      </c>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="6">
-        <v>10</v>
-      </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="11">
-        <v>4</v>
-      </c>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="6">
-        <v>8</v>
-      </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="6">
-        <v>9</v>
-      </c>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="11">
-        <v>15</v>
-      </c>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="23">
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
     <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>